<commit_message>
bubble sort and stack Python
</commit_message>
<xml_diff>
--- a/Interview-Guide.xlsx
+++ b/Interview-Guide.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Topic</t>
   </si>
@@ -109,6 +109,25 @@
   </si>
   <si>
     <t>selection sort nevertakes more then O(n2)</t>
+  </si>
+  <si>
+    <t>Bubble sort</t>
+  </si>
+  <si>
+    <t>pair are compared and sawped for sorting</t>
+  </si>
+  <si>
+    <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>First in Last out
+Last in first out</t>
+  </si>
+  <si>
+    <t>For balancing eqaution it can be used.</t>
   </si>
 </sst>
 </file>
@@ -207,13 +226,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,10 +517,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,34 +536,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="6:11" ht="60" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
@@ -607,20 +626,42 @@
       </c>
     </row>
     <row r="7" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+    <row r="8" spans="6:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F9" s="2"/>

</xml_diff>